<commit_message>
Fixed status extensions.  Added groupings to artifacts page.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-bc-facility-details-extension.xlsx
+++ b/docs/StructureDefinition-bc-facility-details-extension.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$28</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="87">
   <si>
     <t>Path</t>
   </si>
@@ -176,21 +176,11 @@
     <t>Extension.extension</t>
   </si>
   <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
     <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+    <t>An Extension</t>
   </si>
   <si>
     <t xml:space="preserve">value:url}
@@ -212,9 +202,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>An Extension</t>
-  </si>
-  <si>
     <t>Extension.extension.id</t>
   </si>
   <si>
@@ -268,17 +255,30 @@
     <t>contactName</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/ca-bc/provider/StructureDefinition/bc-status-extension}
+    <t>period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/ca-bc/provider/StructureDefinition/bc-period-extension}
 </t>
   </si>
   <si>
-    <t>BC Status Extension</t>
-  </si>
-  <si>
-    <t>Tracking status codes and the effective dates of those statuses.</t>
+    <t>BC Valid Period</t>
+  </si>
+  <si>
+    <t>The period for when the extended element is valid.</t>
+  </si>
+  <si>
+    <t>endReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/ca-bc/provider/StructureDefinition/bc-end-reason-extension}
+</t>
+  </si>
+  <si>
+    <t>BC End Reason Extension</t>
+  </si>
+  <si>
+    <t>Tracking end reasons.</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ca-bc/provider/StructureDefinition/bc-facility-details-extension</t>
@@ -434,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ27"/>
+  <dimension ref="A1:AJ28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -445,7 +445,7 @@
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.08203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.19921875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="8.16796875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
@@ -453,7 +453,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="42.953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="36.2890625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -797,11 +797,11 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s" s="2">
         <v>39</v>
@@ -816,17 +816,15 @@
         <v>37</v>
       </c>
       <c r="J4" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K4" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="L4" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="K4" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="L4" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="M4" t="s" s="2">
-        <v>56</v>
-      </c>
+      <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
         <v>37</v>
@@ -863,19 +861,19 @@
         <v>37</v>
       </c>
       <c r="AA4" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AB4" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AC4" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD4" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AE4" t="s" s="2">
         <v>57</v>
-      </c>
-      <c r="AB4" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AC4" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD4" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AE4" t="s" s="2">
-        <v>60</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>38</v>
@@ -890,7 +888,7 @@
         <v>43</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
@@ -898,7 +896,7 @@
         <v>51</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s" s="2">
         <v>37</v>
@@ -911,7 +909,7 @@
         <v>45</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>37</v>
@@ -920,13 +918,13 @@
         <v>37</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K5" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -977,7 +975,7 @@
         <v>37</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>38</v>
@@ -997,7 +995,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1097,7 +1095,7 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
@@ -1120,13 +1118,13 @@
         <v>37</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K7" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1165,19 +1163,19 @@
         <v>37</v>
       </c>
       <c r="AA7" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AB7" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AC7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD7" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AE7" t="s" s="2">
         <v>57</v>
-      </c>
-      <c r="AB7" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AC7" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD7" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AE7" t="s" s="2">
-        <v>60</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>38</v>
@@ -1197,7 +1195,7 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -1220,16 +1218,16 @@
         <v>37</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -1237,7 +1235,7 @@
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" t="s" s="2">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="R8" t="s" s="2">
         <v>37</v>
@@ -1279,7 +1277,7 @@
         <v>37</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>45</v>
@@ -1294,12 +1292,12 @@
         <v>37</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -1325,10 +1323,10 @@
         <v>46</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1379,7 +1377,7 @@
         <v>37</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>38</v>
@@ -1391,10 +1389,10 @@
         <v>37</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
@@ -1402,7 +1400,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>37</v>
@@ -1415,7 +1413,7 @@
         <v>45</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>37</v>
@@ -1424,13 +1422,13 @@
         <v>37</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K10" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1481,7 +1479,7 @@
         <v>37</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>38</v>
@@ -1501,7 +1499,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -1601,7 +1599,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -1624,13 +1622,13 @@
         <v>37</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1669,19 +1667,19 @@
         <v>37</v>
       </c>
       <c r="AA12" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AB12" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AC12" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD12" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AE12" t="s" s="2">
         <v>57</v>
-      </c>
-      <c r="AB12" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AC12" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD12" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>60</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>38</v>
@@ -1701,7 +1699,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -1724,16 +1722,16 @@
         <v>37</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -1741,7 +1739,7 @@
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" t="s" s="2">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="R13" t="s" s="2">
         <v>37</v>
@@ -1783,7 +1781,7 @@
         <v>37</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>45</v>
@@ -1798,12 +1796,12 @@
         <v>37</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -1829,10 +1827,10 @@
         <v>46</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1883,7 +1881,7 @@
         <v>37</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>38</v>
@@ -1895,10 +1893,10 @@
         <v>37</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -1906,7 +1904,7 @@
         <v>51</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s" s="2">
         <v>37</v>
@@ -1919,7 +1917,7 @@
         <v>45</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>37</v>
@@ -1928,13 +1926,13 @@
         <v>37</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1985,7 +1983,7 @@
         <v>37</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>38</v>
@@ -2005,7 +2003,7 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2105,7 +2103,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2128,13 +2126,13 @@
         <v>37</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K17" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2173,19 +2171,19 @@
         <v>37</v>
       </c>
       <c r="AA17" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AB17" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AC17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD17" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AE17" t="s" s="2">
         <v>57</v>
-      </c>
-      <c r="AB17" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AC17" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD17" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AE17" t="s" s="2">
-        <v>60</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>38</v>
@@ -2205,7 +2203,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2228,16 +2226,16 @@
         <v>37</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -2245,7 +2243,7 @@
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" t="s" s="2">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="R18" t="s" s="2">
         <v>37</v>
@@ -2287,7 +2285,7 @@
         <v>37</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>45</v>
@@ -2302,12 +2300,12 @@
         <v>37</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -2333,10 +2331,10 @@
         <v>46</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2387,7 +2385,7 @@
         <v>37</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>38</v>
@@ -2399,10 +2397,10 @@
         <v>37</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
@@ -2410,7 +2408,7 @@
         <v>51</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s" s="2">
         <v>37</v>
@@ -2423,7 +2421,7 @@
         <v>45</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>37</v>
@@ -2432,13 +2430,13 @@
         <v>37</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K20" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2489,7 +2487,7 @@
         <v>37</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>38</v>
@@ -2509,7 +2507,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -2609,7 +2607,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -2632,13 +2630,13 @@
         <v>37</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K22" t="s" s="2">
         <v>36</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -2677,19 +2675,19 @@
         <v>37</v>
       </c>
       <c r="AA22" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AB22" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AC22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD22" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AE22" t="s" s="2">
         <v>57</v>
-      </c>
-      <c r="AB22" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="AC22" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD22" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AE22" t="s" s="2">
-        <v>60</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>38</v>
@@ -2709,7 +2707,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -2732,16 +2730,16 @@
         <v>37</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -2749,7 +2747,7 @@
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" t="s" s="2">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R23" t="s" s="2">
         <v>37</v>
@@ -2791,7 +2789,7 @@
         <v>37</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>45</v>
@@ -2806,12 +2804,12 @@
         <v>37</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -2837,10 +2835,10 @@
         <v>46</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -2891,7 +2889,7 @@
         <v>37</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>38</v>
@@ -2903,10 +2901,10 @@
         <v>37</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25">
@@ -2914,20 +2912,20 @@
         <v>51</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>37</v>
@@ -2936,13 +2934,13 @@
         <v>37</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2993,7 +2991,7 @@
         <v>37</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>38</v>
@@ -3011,23 +3009,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="B26" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>81</v>
+      </c>
       <c r="C26" t="s" s="2">
         <v>37</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>37</v>
@@ -3036,24 +3036,22 @@
         <v>37</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>70</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>37</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" t="s" s="2">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="R26" t="s" s="2">
         <v>37</v>
@@ -3095,27 +3093,27 @@
         <v>37</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="AH26" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>72</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3123,10 +3121,10 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>37</v>
@@ -3138,22 +3136,24 @@
         <v>37</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="M27" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>66</v>
+      </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>37</v>
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" t="s" s="2">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="R27" t="s" s="2">
         <v>37</v>
@@ -3195,10 +3195,10 @@
         <v>37</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>45</v>
@@ -3207,14 +3207,114 @@
         <v>37</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="AJ27" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" hidden="true">
+      <c r="A28" t="s" s="2">
         <v>72</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J28" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="K28" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P28" s="2"/>
+      <c r="Q28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE28" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AF28" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG28" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AH28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI28" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ27">
+  <autoFilter ref="A1:AJ28">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3224,7 +3324,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI26">
+  <conditionalFormatting sqref="A2:AI27">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>